<commit_message>
small adjustment to X button
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -189,8 +189,8 @@
   </sheetPr>
   <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0" tabSelected="1">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView topLeftCell="A50" workbookViewId="0" tabSelected="1">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -624,6 +624,9 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="13.5">
+      <c r="A73" t="s">
+        <v>0</v>
+      </c>
       <c r="B73" t="inlineStr">
         <is>
           <t>add colors</t>

</xml_diff>

<commit_message>
add admin check to each route handler's callback
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -28,12 +28,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>fix the 127 limit column</t>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>delete coupon</t>
   </si>
   <si>
     <t>admin view</t>
@@ -187,10 +190,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:I73"/>
+  <dimension ref="A2:I96"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0" tabSelected="1">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView topLeftCell="A71" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -590,8 +593,10 @@
       <c r="A57" t="s">
         <v>0</v>
       </c>
-      <c r="B57" t="s">
-        <v>1</v>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>fix the 127 limit column</t>
+        </is>
       </c>
     </row>
     <row r="58" spans="1:9" ht="13.5">
@@ -630,6 +635,73 @@
       <c r="B73" t="inlineStr">
         <is>
           <t>add colors</t>
+        </is>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="13.5">
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="13.5">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="13.5">
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>coupon passes view limit</t>
+        </is>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="13.5">
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2 coupons added to same page</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>one should be rejected</t>
+        </is>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="13.5">
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>old visits not counted towards displayThreshold</t>
+        </is>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="13.5">
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>ensures user is an admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="13.5">
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>wrap up</t>
+        </is>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="13.5">
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>reduce bundle size</t>
+        </is>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="13.5">
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>add option to have a dashed border</t>
         </is>
       </c>
     </row>
@@ -750,7 +822,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -770,10 +842,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>2</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -782,7 +854,7 @@
       </c>
       <c r="G20" s="6"/>
       <c r="I20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K20" s="6" t="inlineStr">
         <is>
@@ -793,10 +865,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -831,16 +903,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" t="s">
         <v>6</v>
       </c>
-      <c r="I26" t="s">
-        <v>5</v>
-      </c>
       <c r="K26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -1768,7 +1840,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -1778,7 +1850,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>

</xml_diff>

<commit_message>
add duplicate target checking, in clauses, snackbar error posting to front end
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -190,10 +190,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:I96"/>
+  <dimension ref="A2:I101"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView topLeftCell="A85" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -702,6 +702,20 @@
       <c r="C96" t="inlineStr">
         <is>
           <t>add option to have a dashed border</t>
+        </is>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="13.5">
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>put cookie ids inside a jwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="13.5">
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>front end styling</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactored to use script localization and enqueuing
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="11500" windowHeight="5700"/>
+    <workbookView activeTab="3" windowWidth="11500" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="todo" sheetId="1" r:id="rId1"/>
@@ -28,15 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>tests</t>
-  </si>
-  <si>
-    <t>delete coupon</t>
   </si>
   <si>
     <t>admin view</t>
@@ -190,10 +184,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:I101"/>
+  <dimension ref="A2:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -203,6 +197,7 @@
     <col min="4" max="4" style="1" width="3.7140625000000003" customWidth="1"/>
     <col min="5" max="5" style="1" width="3.2855168269230774" customWidth="1"/>
     <col min="6" max="256" style="1" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="13.5">
@@ -590,27 +585,9 @@
     </row>
     <row r="55" spans="1:9" ht="13.5"/>
     <row r="57" spans="1:9" ht="13.5">
-      <c r="A57" t="s">
-        <v>0</v>
-      </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>fix the 127 limit column</t>
-        </is>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="13.5">
-      <c r="B58" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>find the right clause</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>alter table... Modify ... (no "column" keyword)</t>
         </is>
       </c>
     </row>
@@ -618,104 +595,6 @@
       <c r="B64" t="inlineStr">
         <is>
           <t>fix the backgrounds only covering text</t>
-        </is>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="13.5">
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>try dropping sql int dlsplay values on the create table statements before running the plugin again</t>
-        </is>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="13.5">
-      <c r="A73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>add colors</t>
-        </is>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="13.5">
-      <c r="B77" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="13.5">
-      <c r="A78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C78" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="13.5">
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>coupon passes view limit</t>
-        </is>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="13.5">
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>2 coupons added to same page</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>one should be rejected</t>
-        </is>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="13.5">
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>old visits not counted towards displayThreshold</t>
-        </is>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="13.5">
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>ensures user is an admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="13.5">
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>wrap up</t>
-        </is>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="13.5">
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>reduce bundle size</t>
-        </is>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="13.5">
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>add option to have a dashed border</t>
-        </is>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="13.5">
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>put cookie ids inside a jwt</t>
-        </is>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="13.5">
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>front end styling</t>
         </is>
       </c>
     </row>
@@ -744,8 +623,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="3" width="9.142307692307693"/>
-    <col min="2" max="256" style="3" width="9.142307692307693"/>
+    <col min="1" max="256" style="3" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -772,8 +651,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.142307692307693"/>
-    <col min="2" max="256" style="4" width="9.142307692307693"/>
+    <col min="1" max="256" style="4" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:6" ht="13.5">
@@ -805,16 +684,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="B5:K233"/>
+  <dimension ref="B5:K242"/>
   <sheetViews>
-    <sheetView topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="B229" sqref="B229"/>
+    <sheetView topLeftCell="A232" workbookViewId="0" tabSelected="1">
+      <selection activeCell="D243" sqref="D243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.142307692307693"/>
-    <col min="2" max="256" style="5" width="9.142307692307693"/>
+    <col min="1" max="256" style="5" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:11" ht="13.5">
@@ -836,7 +715,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -856,10 +735,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -868,7 +747,7 @@
       </c>
       <c r="G20" s="6"/>
       <c r="I20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K20" s="6" t="inlineStr">
         <is>
@@ -879,10 +758,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -917,16 +796,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -1854,7 +1733,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -1864,7 +1743,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>
@@ -1884,6 +1763,34 @@
       <c r="D233" t="inlineStr">
         <is>
           <t>add code for stamping unixTime to new targets and visit records</t>
+        </is>
+      </c>
+    </row>
+    <row r="237" spans="2:11" ht="13.5">
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>register React.js as a "handle" reactAdminArea</t>
+        </is>
+      </c>
+    </row>
+    <row r="238" spans="2:11" ht="13.5">
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>setup a data object and localize it</t>
+        </is>
+      </c>
+    </row>
+    <row r="240" spans="2:11" ht="13.5">
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>enqueue reactAdminArea</t>
+        </is>
+      </c>
+    </row>
+    <row r="242" spans="2:11" ht="13.5">
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>next step is to figure out how to target a specific page doing all this</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor passed variables to be from serverParams object
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="3" windowWidth="11500" windowHeight="5700"/>
+    <workbookView activeTab="0" windowWidth="11500" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="todo" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>delete coupon</t>
   </si>
   <si>
     <t>admin view</t>
@@ -184,10 +187,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:I64"/>
+  <dimension ref="A2:I111"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView topLeftCell="A92" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -197,7 +200,6 @@
     <col min="4" max="4" style="1" width="3.7140625000000003" customWidth="1"/>
     <col min="5" max="5" style="1" width="3.2855168269230774" customWidth="1"/>
     <col min="6" max="256" style="1" width="9.142307692307693"/>
-    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="13.5">
@@ -585,9 +587,27 @@
     </row>
     <row r="55" spans="1:9" ht="13.5"/>
     <row r="57" spans="1:9" ht="13.5">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>fix the 127 limit column</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="13.5">
+      <c r="B58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>find the right clause</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>alter table... Modify ... (no "column" keyword)</t>
         </is>
       </c>
     </row>
@@ -595,6 +615,155 @@
       <c r="B64" t="inlineStr">
         <is>
           <t>fix the backgrounds only covering text</t>
+        </is>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="13.5">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>try dropping sql int dlsplay values on the create table statements before running the plugin again</t>
+        </is>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="13.5">
+      <c r="A73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>add colors</t>
+        </is>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="13.5">
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>tests</t>
+        </is>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="13.5">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="13.5">
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>coupon passes view limit</t>
+        </is>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="13.5">
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2 coupons added to same page</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>one should be rejected</t>
+        </is>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="13.5">
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>old visits not counted towards displayThreshold</t>
+        </is>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="13.5">
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>ensures user is an admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="13.5">
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>setup admin check</t>
+        </is>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="13.5">
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>switch to none verification</t>
+        </is>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="13.5">
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>secure the nonce with a jwt library</t>
+        </is>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="13.5">
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>wrap up</t>
+        </is>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="13.5">
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>reduce bundle size</t>
+        </is>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="13.5">
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>add option to have a dashed border</t>
+        </is>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="13.5">
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>put cookie ids inside a jwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="13.5">
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>front end styling</t>
+        </is>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="13.5">
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>fix stretching way to the right</t>
+        </is>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="13.5">
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>refactor my app injection to use wp functions</t>
+        </is>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="13.5">
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>handle registration</t>
+        </is>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="13.5">
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>php to js variable localization</t>
         </is>
       </c>
     </row>
@@ -623,8 +792,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="256" style="3" width="9.142307692307693"/>
-    <col min="257" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="3" width="9.142307692307693"/>
+    <col min="2" max="256" style="3" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -651,8 +820,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="256" style="4" width="9.142307692307693"/>
-    <col min="257" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="4" width="9.142307692307693"/>
+    <col min="2" max="256" style="4" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:6" ht="13.5">
@@ -684,16 +853,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="B5:K242"/>
+  <dimension ref="B5:K233"/>
   <sheetViews>
-    <sheetView topLeftCell="A232" workbookViewId="0" tabSelected="1">
-      <selection activeCell="D243" sqref="D243"/>
+    <sheetView topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="256" style="5" width="9.142307692307693"/>
-    <col min="257" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="5" width="9.142307692307693"/>
+    <col min="2" max="256" style="5" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:11" ht="13.5">
@@ -715,7 +884,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -735,10 +904,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>1</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -747,7 +916,7 @@
       </c>
       <c r="G20" s="6"/>
       <c r="I20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K20" s="6" t="inlineStr">
         <is>
@@ -758,10 +927,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -796,16 +965,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
         <v>5</v>
       </c>
-      <c r="I26" t="s">
-        <v>4</v>
-      </c>
       <c r="K26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -1733,7 +1902,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -1743,7 +1912,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>
@@ -1763,34 +1932,6 @@
       <c r="D233" t="inlineStr">
         <is>
           <t>add code for stamping unixTime to new targets and visit records</t>
-        </is>
-      </c>
-    </row>
-    <row r="237" spans="2:11" ht="13.5">
-      <c r="D237" t="inlineStr">
-        <is>
-          <t>register React.js as a "handle" reactAdminArea</t>
-        </is>
-      </c>
-    </row>
-    <row r="238" spans="2:11" ht="13.5">
-      <c r="D238" t="inlineStr">
-        <is>
-          <t>setup a data object and localize it</t>
-        </is>
-      </c>
-    </row>
-    <row r="240" spans="2:11" ht="13.5">
-      <c r="D240" t="inlineStr">
-        <is>
-          <t>enqueue reactAdminArea</t>
-        </is>
-      </c>
-    </row>
-    <row r="242" spans="2:11" ht="13.5">
-      <c r="D242" t="inlineStr">
-        <is>
-          <t>next step is to figure out how to target a specific page doing all this</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
remove capitalization on get in the loadAll handler
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -28,12 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>delete coupon</t>
   </si>
   <si>
     <t>admin view</t>
@@ -187,10 +184,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:I111"/>
+  <dimension ref="A2:I118"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView topLeftCell="A100" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -646,8 +643,10 @@
       <c r="A78" t="s">
         <v>0</v>
       </c>
-      <c r="C78" t="s">
-        <v>1</v>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>delete coupon</t>
+        </is>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13.5">
@@ -704,6 +703,9 @@
         </is>
       </c>
     </row>
+    <row r="92" spans="1:9">
+      <c r="C92" s="0"/>
+    </row>
     <row r="94" spans="1:9" ht="13.5">
       <c r="B94" t="inlineStr">
         <is>
@@ -746,7 +748,17 @@
         </is>
       </c>
     </row>
+    <row r="105" spans="1:9" ht="13.5">
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>pass API namespace to the front end</t>
+        </is>
+      </c>
+    </row>
     <row r="109" spans="1:9" ht="13.5">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
       <c r="B109" t="inlineStr">
         <is>
           <t>refactor my app injection to use wp functions</t>
@@ -754,6 +766,9 @@
       </c>
     </row>
     <row r="110" spans="1:9" ht="13.5">
+      <c r="A110" t="s">
+        <v>0</v>
+      </c>
       <c r="C110" t="inlineStr">
         <is>
           <t>handle registration</t>
@@ -761,9 +776,62 @@
       </c>
     </row>
     <row r="111" spans="1:9" ht="13.5">
+      <c r="A111" t="s">
+        <v>0</v>
+      </c>
       <c r="C111" t="inlineStr">
         <is>
           <t>php to js variable localization</t>
+        </is>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="13.5">
+      <c r="A112" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>enqueuing script</t>
+        </is>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="13.5">
+      <c r="A113" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>adding action to do all this</t>
+        </is>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="13.5">
+      <c r="A115" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>another function to create a div</t>
+        </is>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="13.5">
+      <c r="A116" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>another action to bind it to the admin footer, i guess right before &lt;/ body&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="13.5">
+      <c r="A118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>solving the issue with babel-polyfill running twice</t>
         </is>
       </c>
     </row>
@@ -884,7 +952,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -904,10 +972,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -916,7 +984,7 @@
       </c>
       <c r="G20" s="6"/>
       <c r="I20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K20" s="6" t="inlineStr">
         <is>
@@ -927,10 +995,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -965,16 +1033,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>5</v>
       </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
       <c r="I26" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" t="s">
         <v>5</v>
-      </c>
-      <c r="K26" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -1902,7 +1970,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -1912,7 +1980,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>

</xml_diff>

<commit_message>
add jwt encoding and decoding into the get and create cookie methods in the Visitors class
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="11500" windowHeight="5700"/>
+    <workbookView activeTab="3" windowWidth="11500" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="todo" sheetId="1" r:id="rId1"/>
@@ -184,10 +184,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:I118"/>
+  <dimension ref="A2:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -197,6 +197,7 @@
     <col min="4" max="4" style="1" width="3.7140625000000003" customWidth="1"/>
     <col min="5" max="5" style="1" width="3.2855168269230774" customWidth="1"/>
     <col min="6" max="256" style="1" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="13.5">
@@ -584,27 +585,9 @@
     </row>
     <row r="55" spans="1:9" ht="13.5"/>
     <row r="57" spans="1:9" ht="13.5">
-      <c r="A57" t="s">
-        <v>0</v>
-      </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>fix the 127 limit column</t>
-        </is>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="13.5">
-      <c r="B58" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>find the right clause</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>alter table... Modify ... (no "column" keyword)</t>
         </is>
       </c>
     </row>
@@ -612,226 +595,6 @@
       <c r="B64" t="inlineStr">
         <is>
           <t>fix the backgrounds only covering text</t>
-        </is>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="13.5">
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>try dropping sql int dlsplay values on the create table statements before running the plugin again</t>
-        </is>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="13.5">
-      <c r="A73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>add colors</t>
-        </is>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="13.5">
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>tests</t>
-        </is>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="13.5">
-      <c r="A78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>delete coupon</t>
-        </is>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="13.5">
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>coupon passes view limit</t>
-        </is>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="13.5">
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>2 coupons added to same page</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>one should be rejected</t>
-        </is>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="13.5">
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>old visits not counted towards displayThreshold</t>
-        </is>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="13.5">
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>ensures user is an admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="13.5">
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>setup admin check</t>
-        </is>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="13.5">
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>switch to none verification</t>
-        </is>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="13.5">
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>secure the nonce with a jwt library</t>
-        </is>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="C92" s="0"/>
-    </row>
-    <row r="94" spans="1:9" ht="13.5">
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>wrap up</t>
-        </is>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="13.5">
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>reduce bundle size</t>
-        </is>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="13.5">
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>add option to have a dashed border</t>
-        </is>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="13.5">
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>put cookie ids inside a jwt</t>
-        </is>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="13.5">
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>front end styling</t>
-        </is>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="13.5">
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>fix stretching way to the right</t>
-        </is>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="13.5">
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>pass API namespace to the front end</t>
-        </is>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="13.5">
-      <c r="A109" t="s">
-        <v>0</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>refactor my app injection to use wp functions</t>
-        </is>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="13.5">
-      <c r="A110" t="s">
-        <v>0</v>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>handle registration</t>
-        </is>
-      </c>
-    </row>
-    <row r="111" spans="1:9" ht="13.5">
-      <c r="A111" t="s">
-        <v>0</v>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>php to js variable localization</t>
-        </is>
-      </c>
-    </row>
-    <row r="112" spans="1:9" ht="13.5">
-      <c r="A112" t="s">
-        <v>0</v>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>enqueuing script</t>
-        </is>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="13.5">
-      <c r="A113" t="s">
-        <v>0</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>adding action to do all this</t>
-        </is>
-      </c>
-    </row>
-    <row r="115" spans="1:9" ht="13.5">
-      <c r="A115" t="s">
-        <v>0</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>another function to create a div</t>
-        </is>
-      </c>
-    </row>
-    <row r="116" spans="1:9" ht="13.5">
-      <c r="A116" t="s">
-        <v>0</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>another action to bind it to the admin footer, i guess right before &lt;/ body&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="118" spans="1:9" ht="13.5">
-      <c r="A118" t="s">
-        <v>0</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>solving the issue with babel-polyfill running twice</t>
         </is>
       </c>
     </row>
@@ -860,8 +623,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="3" width="9.142307692307693"/>
-    <col min="2" max="256" style="3" width="9.142307692307693"/>
+    <col min="1" max="256" style="3" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -888,8 +651,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.142307692307693"/>
-    <col min="2" max="256" style="4" width="9.142307692307693"/>
+    <col min="1" max="256" style="4" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:6" ht="13.5">
@@ -921,16 +684,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="B5:K233"/>
+  <dimension ref="B5:K250"/>
   <sheetViews>
-    <sheetView topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="B229" sqref="B229"/>
+    <sheetView topLeftCell="A239" workbookViewId="0" tabSelected="1">
+      <selection activeCell="D251" sqref="D251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.142307692307693"/>
-    <col min="2" max="256" style="5" width="9.142307692307693"/>
+    <col min="1" max="256" style="5" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:11" ht="13.5">
@@ -2003,6 +1766,62 @@
         </is>
       </c>
     </row>
+    <row r="237" spans="2:11" ht="13.5">
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>register React.js as a "handle" reactAdminArea</t>
+        </is>
+      </c>
+    </row>
+    <row r="238" spans="2:11" ht="13.5">
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>setup a data object and localize it</t>
+        </is>
+      </c>
+    </row>
+    <row r="240" spans="2:11" ht="13.5">
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>enqueue reactAdminArea</t>
+        </is>
+      </c>
+    </row>
+    <row r="242" spans="2:11" ht="13.5">
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>next step is to figure out how to target a specific page doing all this</t>
+        </is>
+      </c>
+    </row>
+    <row r="246" spans="2:11" ht="13.5">
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>jwt library</t>
+        </is>
+      </c>
+    </row>
+    <row r="247" spans="2:11" ht="13.5">
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>encodes on the cookie setter</t>
+        </is>
+      </c>
+    </row>
+    <row r="248" spans="2:11" ht="13.5">
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>decodes in the apiController class</t>
+        </is>
+      </c>
+    </row>
+    <row r="250" spans="2:11" ht="13.5">
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>importing</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>

</xml_diff>

<commit_message>
draft jwt nonce encode/decode
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="3" windowWidth="11500" windowHeight="5700"/>
+    <workbookView activeTab="0" windowWidth="11500" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="todo" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>setup admin check</t>
+  </si>
+  <si>
+    <t>switch to nonce verification</t>
   </si>
   <si>
     <t>admin view</t>
@@ -150,7 +156,7 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -158,6 +164,9 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0">
@@ -184,10 +193,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:I64"/>
+  <dimension ref="A2:I118"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView topLeftCell="A79" workbookViewId="0" tabSelected="1">
+      <selection activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -197,7 +206,6 @@
     <col min="4" max="4" style="1" width="3.7140625000000003" customWidth="1"/>
     <col min="5" max="5" style="1" width="3.2855168269230774" customWidth="1"/>
     <col min="6" max="256" style="1" width="9.142307692307693"/>
-    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="13.5">
@@ -585,9 +593,27 @@
     </row>
     <row r="55" spans="1:9" ht="13.5"/>
     <row r="57" spans="1:9" ht="13.5">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>fix the 127 limit column</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="13.5">
+      <c r="B58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>find the right clause</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>alter table... Modify ... (no "column" keyword)</t>
         </is>
       </c>
     </row>
@@ -595,6 +621,230 @@
       <c r="B64" t="inlineStr">
         <is>
           <t>fix the backgrounds only covering text</t>
+        </is>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="13.5">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>try dropping sql int dlsplay values on the create table statements before running the plugin again</t>
+        </is>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="13.5">
+      <c r="A73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>add colors</t>
+        </is>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="13.5">
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>tests</t>
+        </is>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="13.5">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>delete coupon</t>
+        </is>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="13.5">
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>coupon passes view limit</t>
+        </is>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="13.5">
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2 coupons added to same page</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>one should be rejected</t>
+        </is>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="13.5">
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>old visits not counted towards displayThreshold</t>
+        </is>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="13.5">
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>ensures user is an admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="13.5">
+      <c r="A87" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="13.5">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>///////////</t>
+        </is>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="13.5">
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>secure the nonce with a jwt library</t>
+        </is>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="13.5">
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>wrap up</t>
+        </is>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="13.5">
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>reduce bundle size</t>
+        </is>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="13.5">
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>add option to have a dashed border</t>
+        </is>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="13.5">
+      <c r="A98" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>put cookie ids inside a jwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="13.5">
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>front end styling</t>
+        </is>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="13.5">
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>fix stretching way to the right</t>
+        </is>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="13.5">
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>pass API namespace to the front end</t>
+        </is>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="13.5">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>refactor my app injection to use wp functions</t>
+        </is>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="13.5">
+      <c r="A110" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>handle registration</t>
+        </is>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="13.5">
+      <c r="A111" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>php to js variable localization</t>
+        </is>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="13.5">
+      <c r="A112" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>enqueuing script</t>
+        </is>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="13.5">
+      <c r="A113" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>adding action to do all this</t>
+        </is>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="13.5">
+      <c r="A115" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>another function to create a div</t>
+        </is>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="13.5">
+      <c r="A116" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>another action to bind it to the admin footer, i guess right before &lt;/ body&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="13.5">
+      <c r="A118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>solving the issue with babel-polyfill running twice</t>
         </is>
       </c>
     </row>
@@ -623,8 +873,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="256" style="3" width="9.142307692307693"/>
-    <col min="257" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="4" width="9.142307692307693"/>
+    <col min="2" max="256" style="4" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -651,8 +901,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="256" style="4" width="9.142307692307693"/>
-    <col min="257" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="5" width="9.142307692307693"/>
+    <col min="2" max="256" style="5" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:6" ht="13.5">
@@ -684,16 +934,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="B5:K250"/>
+  <dimension ref="B5:K233"/>
   <sheetViews>
-    <sheetView topLeftCell="A239" workbookViewId="0" tabSelected="1">
-      <selection activeCell="D251" sqref="D251"/>
+    <sheetView topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="256" style="5" width="9.142307692307693"/>
-    <col min="257" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="6" width="9.142307692307693"/>
+    <col min="2" max="256" style="6" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:11" ht="13.5">
@@ -715,7 +965,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -735,21 +985,21 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>out</t>
         </is>
       </c>
-      <c r="G20" s="6"/>
+      <c r="G20" s="7"/>
       <c r="I20" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" s="6" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="K20" s="7" t="inlineStr">
         <is>
           <t>see current coupons view</t>
         </is>
@@ -758,10 +1008,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K22" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -796,16 +1046,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K26" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -981,7 +1231,7 @@
       </c>
     </row>
     <row r="77" spans="2:11" ht="13.5">
-      <c r="C77" s="6" t="inlineStr">
+      <c r="C77" s="7" t="inlineStr">
         <is>
           <t>send row delete request</t>
         </is>
@@ -1026,7 +1276,7 @@
     <row r="81" spans="2:11" ht="13.5"/>
     <row r="82" spans="2:11" ht="13.5"/>
     <row r="83" spans="2:11" ht="13.5">
-      <c r="C83" s="6" t="inlineStr">
+      <c r="C83" s="7" t="inlineStr">
         <is>
           <t>load coupon data</t>
         </is>
@@ -1061,7 +1311,7 @@
       </c>
     </row>
     <row r="88" spans="2:11" ht="13.5">
-      <c r="C88" s="7" t="inlineStr">
+      <c r="C88" s="8" t="inlineStr">
         <is>
           <t>implementation</t>
         </is>
@@ -1122,7 +1372,7 @@
     <row r="95" spans="2:11" ht="13.5"/>
     <row r="96" spans="2:11" ht="13.5"/>
     <row r="97" spans="2:11" ht="13.5">
-      <c r="C97" s="6" t="inlineStr">
+      <c r="C97" s="7" t="inlineStr">
         <is>
           <t>receive a global variable from php into my javascript bundle file</t>
         </is>
@@ -1160,7 +1410,7 @@
     <row r="103" spans="2:11" ht="13.5"/>
     <row r="104" spans="2:11" ht="13.5"/>
     <row r="105" spans="2:11" ht="13.5">
-      <c r="C105" s="6" t="inlineStr">
+      <c r="C105" s="7" t="inlineStr">
         <is>
           <t>set up db fixtures for dev mode that work with production</t>
         </is>
@@ -1204,7 +1454,7 @@
     <row r="111" spans="2:11" ht="13.5"/>
     <row r="112" spans="2:11" ht="13.5"/>
     <row r="113" spans="2:11" ht="13.5">
-      <c r="C113" s="6" t="inlineStr">
+      <c r="C113" s="7" t="inlineStr">
         <is>
           <t>wiring the post requestor up</t>
         </is>
@@ -1237,7 +1487,7 @@
       </c>
     </row>
     <row r="120" spans="2:11">
-      <c r="C120" s="6" t="inlineStr">
+      <c r="C120" s="7" t="inlineStr">
         <is>
           <t>ajaxControllers for the admin area</t>
         </is>
@@ -1320,7 +1570,7 @@
       </c>
     </row>
     <row r="139" spans="2:11" ht="13.5">
-      <c r="C139" s="6" t="inlineStr">
+      <c r="C139" s="7" t="inlineStr">
         <is>
           <t>Create table</t>
         </is>
@@ -1555,7 +1805,7 @@
     <row r="180" spans="2:11" ht="13.5"/>
     <row r="181" spans="2:11" ht="13.5"/>
     <row r="182" spans="2:11" ht="13.5">
-      <c r="C182" s="6" t="inlineStr">
+      <c r="C182" s="7" t="inlineStr">
         <is>
           <t>visitor cookie setting and getting</t>
         </is>
@@ -1733,7 +1983,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -1743,7 +1993,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>
@@ -1763,62 +2013,6 @@
       <c r="D233" t="inlineStr">
         <is>
           <t>add code for stamping unixTime to new targets and visit records</t>
-        </is>
-      </c>
-    </row>
-    <row r="237" spans="2:11" ht="13.5">
-      <c r="D237" t="inlineStr">
-        <is>
-          <t>register React.js as a "handle" reactAdminArea</t>
-        </is>
-      </c>
-    </row>
-    <row r="238" spans="2:11" ht="13.5">
-      <c r="D238" t="inlineStr">
-        <is>
-          <t>setup a data object and localize it</t>
-        </is>
-      </c>
-    </row>
-    <row r="240" spans="2:11" ht="13.5">
-      <c r="D240" t="inlineStr">
-        <is>
-          <t>enqueue reactAdminArea</t>
-        </is>
-      </c>
-    </row>
-    <row r="242" spans="2:11" ht="13.5">
-      <c r="D242" t="inlineStr">
-        <is>
-          <t>next step is to figure out how to target a specific page doing all this</t>
-        </is>
-      </c>
-    </row>
-    <row r="246" spans="2:11" ht="13.5">
-      <c r="D246" t="inlineStr">
-        <is>
-          <t>jwt library</t>
-        </is>
-      </c>
-    </row>
-    <row r="247" spans="2:11" ht="13.5">
-      <c r="D247" t="inlineStr">
-        <is>
-          <t>encodes on the cookie setter</t>
-        </is>
-      </c>
-    </row>
-    <row r="248" spans="2:11" ht="13.5">
-      <c r="D248" t="inlineStr">
-        <is>
-          <t>decodes in the apiController class</t>
-        </is>
-      </c>
-    </row>
-    <row r="250" spans="2:11" ht="13.5">
-      <c r="D250" t="inlineStr">
-        <is>
-          <t>importing</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
successful test of json encode and decode
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -195,8 +195,8 @@
   </sheetPr>
   <dimension ref="A2:I118"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0" tabSelected="1">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView topLeftCell="A86" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -744,6 +744,13 @@
       <c r="C98" t="inlineStr">
         <is>
           <t>put cookie ids inside a jwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="13.5">
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>rename the visitorId cookie to something more proprietary</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
change cookie to namespaced name
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -193,10 +193,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:I118"/>
+  <dimension ref="A2:I124"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView topLeftCell="A107" workbookViewId="0" tabSelected="1">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -852,6 +852,16 @@
       <c r="B118" t="inlineStr">
         <is>
           <t>solving the issue with babel-polyfill running twice</t>
+        </is>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="13.5">
+      <c r="A124" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>remove nonce encryption</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
wip sending api namespace to front end
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -195,8 +195,8 @@
   </sheetPr>
   <dimension ref="A2:I124"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" workbookViewId="0" tabSelected="1">
-      <selection activeCell="F120" sqref="F120"/>
+    <sheetView topLeftCell="A86" workbookViewId="0" tabSelected="1">
+      <selection activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -748,6 +748,9 @@
       </c>
     </row>
     <row r="99" spans="1:9" ht="13.5">
+      <c r="A99" t="s">
+        <v>0</v>
+      </c>
       <c r="C99" t="inlineStr">
         <is>
           <t>rename the visitorId cookie to something more proprietary</t>

</xml_diff>

<commit_message>
send namespace from back end completed on both sides
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -28,9 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
   <si>
     <t>setup admin check</t>
@@ -196,7 +199,7 @@
   <dimension ref="A2:I124"/>
   <sheetViews>
     <sheetView topLeftCell="A86" workbookViewId="0" tabSelected="1">
-      <selection activeCell="K94" sqref="K94"/>
+      <selection activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -475,10 +478,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="13.5">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
+      <c r="A33" t="s">
+        <v>1</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -696,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="13.5">
@@ -706,7 +707,7 @@
         </is>
       </c>
       <c r="D88" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="13.5">
@@ -772,6 +773,9 @@
       </c>
     </row>
     <row r="105" spans="1:9" ht="13.5">
+      <c r="A105" t="s">
+        <v>1</v>
+      </c>
       <c r="C105" t="inlineStr">
         <is>
           <t>pass API namespace to the front end</t>
@@ -985,7 +989,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -1005,10 +1009,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1017,7 +1021,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="I20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K20" s="7" t="inlineStr">
         <is>
@@ -1028,10 +1032,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -1066,16 +1070,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
         <v>7</v>
       </c>
-      <c r="I26" t="s">
-        <v>6</v>
-      </c>
       <c r="K26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -2003,7 +2007,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -2013,7 +2017,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>

</xml_diff>

<commit_message>
add indent for wp left side menu
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="11500" windowHeight="5700"/>
+    <workbookView activeTab="3" windowWidth="11500" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="todo" sheetId="1" r:id="rId1"/>
@@ -28,18 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>/</t>
-  </si>
-  <si>
-    <t>setup admin check</t>
-  </si>
-  <si>
-    <t>switch to nonce verification</t>
   </si>
   <si>
     <t>admin view</t>
@@ -198,7 +192,7 @@
   </sheetPr>
   <dimension ref="A2:I124"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0" tabSelected="1">
+    <sheetView topLeftCell="A86" workbookViewId="0">
       <selection activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
@@ -209,6 +203,7 @@
     <col min="4" max="4" style="1" width="3.7140625000000003" customWidth="1"/>
     <col min="5" max="5" style="1" width="3.2855168269230774" customWidth="1"/>
     <col min="6" max="256" style="1" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="13.5">
@@ -696,8 +691,10 @@
       <c r="A87" t="s">
         <v>0</v>
       </c>
-      <c r="D87" t="s">
-        <v>2</v>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>setup admin check</t>
+        </is>
       </c>
     </row>
     <row r="88" spans="1:9" ht="13.5">
@@ -706,8 +703,10 @@
           <t>///////////</t>
         </is>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>3</v>
+      <c r="D88" s="3" t="inlineStr">
+        <is>
+          <t>switch to nonce verification</t>
+        </is>
       </c>
     </row>
     <row r="89" spans="1:9" ht="13.5">
@@ -897,8 +896,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.142307692307693"/>
-    <col min="2" max="256" style="4" width="9.142307692307693"/>
+    <col min="1" max="256" style="4" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -925,8 +924,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.142307692307693"/>
-    <col min="2" max="256" style="5" width="9.142307692307693"/>
+    <col min="1" max="256" style="5" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:6" ht="13.5">
@@ -958,16 +957,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="B5:K233"/>
+  <dimension ref="B5:K241"/>
   <sheetViews>
-    <sheetView topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="B229" sqref="B229"/>
+    <sheetView topLeftCell="A232" workbookViewId="0" tabSelected="1">
+      <selection activeCell="D242" sqref="D242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="6" width="9.142307692307693"/>
-    <col min="2" max="256" style="6" width="9.142307692307693"/>
+    <col min="1" max="256" style="6" width="9.142307692307693"/>
+    <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:11" ht="13.5">
@@ -989,7 +988,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -1009,10 +1008,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1021,7 +1020,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="I20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K20" s="7" t="inlineStr">
         <is>
@@ -1032,10 +1031,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -1070,16 +1069,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -2007,7 +2006,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -2017,7 +2016,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>
@@ -2037,6 +2036,32 @@
       <c r="D233" t="inlineStr">
         <is>
           <t>add code for stamping unixTime to new targets and visit records</t>
+        </is>
+      </c>
+    </row>
+    <row r="238" spans="2:11" ht="13.5">
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>innerWidth</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>onResize</t>
+        </is>
+      </c>
+    </row>
+    <row r="240" spans="2:11" ht="13.5">
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>push it to state variable</t>
+        </is>
+      </c>
+    </row>
+    <row r="241" spans="2:11" ht="13.5">
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>sc reads the variable and decides left margin based on it</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix add coupon error re: border option blocking new addition
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -190,10 +190,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:I131"/>
+  <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0" tabSelected="1">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView topLeftCell="A128" workbookViewId="0" tabSelected="1">
+      <selection activeCell="J143" sqref="J143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -206,7 +206,7 @@
     <col min="257" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="13.5">
+    <row r="2" spans="1:10" ht="13.5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -216,7 +216,7 @@
         </is>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13.5">
+    <row r="3" spans="1:10" ht="13.5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -226,7 +226,7 @@
         </is>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.5">
+    <row r="4" spans="1:10" ht="13.5">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -236,7 +236,7 @@
         </is>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13.5">
+    <row r="5" spans="1:10" ht="13.5">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -246,7 +246,7 @@
         </is>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.5">
+    <row r="6" spans="1:10" ht="13.5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -256,9 +256,9 @@
         </is>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13.5"/>
-    <row r="8" spans="1:9" ht="13.5"/>
-    <row r="9" spans="1:9" ht="13.5">
+    <row r="7" spans="1:10" ht="13.5"/>
+    <row r="8" spans="1:10" ht="13.5"/>
+    <row r="9" spans="1:10" ht="13.5">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -273,7 +273,7 @@
         </is>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.5">
+    <row r="10" spans="1:10" ht="13.5">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -283,7 +283,7 @@
         </is>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="13.5">
+    <row r="11" spans="1:10" ht="13.5">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -293,15 +293,15 @@
         </is>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="13.5"/>
-    <row r="13" spans="1:9" ht="13.5">
+    <row r="12" spans="1:10" ht="13.5"/>
+    <row r="13" spans="1:10" ht="13.5">
       <c r="B13" t="inlineStr">
         <is>
           <t>build out the html for the settings page</t>
         </is>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="13.5">
+    <row r="14" spans="1:10" ht="13.5">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -311,14 +311,14 @@
         </is>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="13.5">
+    <row r="15" spans="1:10" ht="13.5">
       <c r="C15" t="inlineStr">
         <is>
           <t>current coupons tab</t>
         </is>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="13.5">
+    <row r="16" spans="1:10" ht="13.5">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -328,14 +328,14 @@
         </is>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="13.5">
+    <row r="17" spans="1:10" ht="13.5">
       <c r="D17" t="inlineStr">
         <is>
           <t>formViewContainer</t>
         </is>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.5">
+    <row r="18" spans="1:10" ht="13.5">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -346,7 +346,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="13.5">
+    <row r="19" spans="1:10" ht="13.5">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -356,7 +356,7 @@
         </is>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="13.5">
+    <row r="20" spans="1:10" ht="13.5">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -367,14 +367,14 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="13.5">
+    <row r="21" spans="1:10" ht="13.5">
       <c r="C21" t="inlineStr">
         <is>
           <t>wire the ajaxRequestor into the axios post calls</t>
         </is>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13.5">
+    <row r="22" spans="1:10" ht="13.5">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -384,15 +384,15 @@
         </is>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="13.5"/>
-    <row r="24" spans="1:9" ht="13.5">
+    <row r="23" spans="1:10" ht="13.5"/>
+    <row r="24" spans="1:10" ht="13.5">
       <c r="C24" t="inlineStr">
         <is>
           <t>phpunit</t>
         </is>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="13.5">
+    <row r="25" spans="1:10" ht="13.5">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -402,7 +402,7 @@
         </is>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="13.5">
+    <row r="26" spans="1:10" ht="13.5">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -412,7 +412,7 @@
         </is>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="13.5">
+    <row r="27" spans="1:10" ht="13.5">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -422,7 +422,7 @@
         </is>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="13.5">
+    <row r="28" spans="1:10" ht="13.5">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -432,7 +432,7 @@
         </is>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="13.5">
+    <row r="29" spans="1:10" ht="13.5">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -442,7 +442,7 @@
         </is>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="13.5">
+    <row r="30" spans="1:10" ht="13.5">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -452,7 +452,7 @@
         </is>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="13.5">
+    <row r="31" spans="1:10" ht="13.5">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -462,7 +462,7 @@
         </is>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="13.5">
+    <row r="32" spans="1:10" ht="13.5">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -472,7 +472,7 @@
         </is>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="13.5">
+    <row r="33" spans="1:10" ht="13.5">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -487,14 +487,14 @@
         </is>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="13.5">
+    <row r="34" spans="1:10" ht="13.5">
       <c r="C34" t="inlineStr">
         <is>
           <t>db testing</t>
         </is>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="13.5">
+    <row r="35" spans="1:10" ht="13.5">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -504,38 +504,38 @@
         </is>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="13.5">
+    <row r="36" spans="1:10" ht="13.5">
       <c r="D36" t="inlineStr">
         <is>
           <t>do a loadCouponData() query through the app</t>
         </is>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="13.5">
+    <row r="37" spans="1:10" ht="13.5">
       <c r="D37" t="inlineStr">
         <is>
           <t>fix the auto-loading problem (probably re: async iife)</t>
         </is>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="13.5"/>
-    <row r="39" spans="1:9" ht="13.5">
+    <row r="38" spans="1:10" ht="13.5"/>
+    <row r="39" spans="1:10" ht="13.5">
       <c r="D39" t="inlineStr">
         <is>
           <t>do a manual delete query</t>
         </is>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="13.5"/>
-    <row r="41" spans="1:9" ht="13.5"/>
-    <row r="42" spans="1:9" ht="13.5">
+    <row r="40" spans="1:10" ht="13.5"/>
+    <row r="41" spans="1:10" ht="13.5"/>
+    <row r="42" spans="1:10" ht="13.5">
       <c r="C42" t="inlineStr">
         <is>
           <t>integrate fe and be</t>
         </is>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="13.5">
+    <row r="43" spans="1:10" ht="13.5">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -545,7 +545,7 @@
         </is>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="13.5">
+    <row r="44" spans="1:10" ht="13.5">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -555,7 +555,7 @@
         </is>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="13.5">
+    <row r="45" spans="1:10" ht="13.5">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         </is>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -575,7 +575,7 @@
         </is>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:10">
       <c r="A47" t="inlineStr">
         <is>
           <t>c</t>
@@ -587,8 +587,8 @@
         </is>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="13.5"/>
-    <row r="57" spans="1:9" ht="13.5">
+    <row r="55" spans="1:10" ht="13.5"/>
+    <row r="57" spans="1:10" ht="13.5">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -598,7 +598,7 @@
         </is>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13.5">
+    <row r="58" spans="1:10" ht="13.5">
       <c r="B58" t="s">
         <v>0</v>
       </c>
@@ -613,21 +613,21 @@
         </is>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="13.5">
+    <row r="64" spans="1:10" ht="13.5">
       <c r="B64" t="inlineStr">
         <is>
           <t>fix the backgrounds only covering text</t>
         </is>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="13.5">
+    <row r="70" spans="1:10" ht="13.5">
       <c r="B70" t="inlineStr">
         <is>
           <t>try dropping sql int dlsplay values on the create table statements before running the plugin again</t>
         </is>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="13.5">
+    <row r="73" spans="1:10" ht="13.5">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -637,14 +637,14 @@
         </is>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="13.5">
+    <row r="77" spans="1:10" ht="13.5">
       <c r="B77" t="inlineStr">
         <is>
           <t>tests</t>
         </is>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="13.5">
+    <row r="78" spans="1:10" ht="13.5">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -654,14 +654,14 @@
         </is>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="13.5">
+    <row r="80" spans="1:10" ht="13.5">
       <c r="C80" t="inlineStr">
         <is>
           <t>coupon passes view limit</t>
         </is>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="13.5">
+    <row r="82" spans="1:10" ht="13.5">
       <c r="C82" t="inlineStr">
         <is>
           <t>2 coupons added to same page</t>
@@ -673,21 +673,21 @@
         </is>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="13.5">
+    <row r="84" spans="1:10" ht="13.5">
       <c r="C84" t="inlineStr">
         <is>
           <t>old visits not counted towards displayThreshold</t>
         </is>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="13.5">
+    <row r="86" spans="1:10" ht="13.5">
       <c r="C86" t="inlineStr">
         <is>
           <t>ensures user is an admin</t>
         </is>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="13.5">
+    <row r="87" spans="1:10" ht="13.5">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -697,7 +697,7 @@
         </is>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="13.5">
+    <row r="88" spans="1:10" ht="13.5">
       <c r="A88" t="inlineStr">
         <is>
           <t>///////////</t>
@@ -709,28 +709,28 @@
         </is>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="13.5">
+    <row r="89" spans="1:10" ht="13.5">
       <c r="D89" t="inlineStr">
         <is>
           <t>secure the nonce with a jwt library</t>
         </is>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="13.5">
+    <row r="94" spans="1:10" ht="13.5">
       <c r="B94" t="inlineStr">
         <is>
           <t>wrap up</t>
         </is>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="13.5">
+    <row r="95" spans="1:10" ht="13.5">
       <c r="C95" t="inlineStr">
         <is>
           <t>reduce bundle size</t>
         </is>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="13.5">
+    <row r="96" spans="1:10" ht="13.5">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -740,7 +740,7 @@
         </is>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="13.5">
+    <row r="98" spans="1:10" ht="13.5">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -750,7 +750,7 @@
         </is>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="13.5">
+    <row r="99" spans="1:10" ht="13.5">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -760,14 +760,14 @@
         </is>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="13.5">
+    <row r="101" spans="1:10" ht="13.5">
       <c r="C101" t="inlineStr">
         <is>
           <t>front end styling</t>
         </is>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="13.5">
+    <row r="103" spans="1:10" ht="13.5">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -777,7 +777,7 @@
         </is>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="13.5">
+    <row r="104" spans="1:10" ht="13.5">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -787,7 +787,7 @@
         </is>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="13.5">
+    <row r="105" spans="1:10" ht="13.5">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -797,9 +797,9 @@
         </is>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="13.5">
+    <row r="112" spans="1:10" ht="13.5">
       <c r="A112" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -807,7 +807,7 @@
         </is>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="13.5">
+    <row r="116" spans="1:10" ht="13.5">
       <c r="A116" t="s">
         <v>0</v>
       </c>
@@ -817,7 +817,7 @@
         </is>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="13.5">
+    <row r="117" spans="1:10" ht="13.5">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -827,7 +827,7 @@
         </is>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="13.5">
+    <row r="118" spans="1:10" ht="13.5">
       <c r="A118" t="s">
         <v>0</v>
       </c>
@@ -837,7 +837,7 @@
         </is>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="13.5">
+    <row r="119" spans="1:10" ht="13.5">
       <c r="A119" t="s">
         <v>0</v>
       </c>
@@ -847,7 +847,7 @@
         </is>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="13.5">
+    <row r="120" spans="1:10" ht="13.5">
       <c r="A120" t="s">
         <v>0</v>
       </c>
@@ -857,7 +857,7 @@
         </is>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="13.5">
+    <row r="122" spans="1:10" ht="13.5">
       <c r="A122" t="s">
         <v>0</v>
       </c>
@@ -867,7 +867,7 @@
         </is>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="13.5">
+    <row r="123" spans="1:10" ht="13.5">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -877,7 +877,7 @@
         </is>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="13.5">
+    <row r="125" spans="1:10" ht="13.5">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -887,13 +887,102 @@
         </is>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="13.5">
+    <row r="131" spans="1:10" ht="13.5">
       <c r="A131" t="s">
         <v>0</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
           <t>remove nonce encryption</t>
+        </is>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="13.5">
+      <c r="A136" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>add coupon border option</t>
+        </is>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="13.5">
+      <c r="A137" t="s">
+        <v>0</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>add checkbox</t>
+        </is>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="13.5">
+      <c r="A138" t="s">
+        <v>0</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>add label</t>
+        </is>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="13.5">
+      <c r="A139" t="s">
+        <v>0</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>add state</t>
+        </is>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="13.5">
+      <c r="A140" t="s">
+        <v>0</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>add state to post request</t>
+        </is>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="13.5">
+      <c r="A141" t="s">
+        <v>0</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>create hasBorder column in coupons table</t>
+        </is>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="13.5">
+      <c r="A142" t="s">
+        <v>0</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>add it to create table statement</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>not tested working though</t>
+        </is>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="13.5">
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>set the render template to load the border only if hasBorder is true</t>
+        </is>
+      </c>
+    </row>
+    <row r="148" spans="1:10" ht="13.5">
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>move my view into get_template_part()</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix delete route to have auth AND stop infinite loop due to new object refs
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -190,10 +190,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:J148"/>
+  <dimension ref="A2:J153"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" workbookViewId="0" tabSelected="1">
-      <selection activeCell="J143" sqref="J143"/>
+    <sheetView topLeftCell="A135" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -681,6 +681,9 @@
       </c>
     </row>
     <row r="86" spans="1:10" ht="13.5">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
       <c r="C86" t="inlineStr">
         <is>
           <t>ensures user is an admin</t>
@@ -693,26 +696,18 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>setup admin check</t>
+          <t>pass nonce to X-WP-Nonce</t>
         </is>
       </c>
     </row>
     <row r="88" spans="1:10" ht="13.5">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>///////////</t>
-        </is>
-      </c>
-      <c r="D88" s="3" t="inlineStr">
-        <is>
-          <t>switch to nonce verification</t>
-        </is>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="13.5">
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>secure the nonce with a jwt library</t>
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="1:10" ht="13.5"/>
+    <row r="90" spans="1:10" ht="13.5">
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>add border radius</t>
         </is>
       </c>
     </row>
@@ -732,7 +727,7 @@
     </row>
     <row r="96" spans="1:10" ht="13.5">
       <c r="A96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -973,16 +968,41 @@
       </c>
     </row>
     <row r="143" spans="1:10" ht="13.5">
+      <c r="A143" t="s">
+        <v>0</v>
+      </c>
       <c r="C143" t="inlineStr">
         <is>
           <t>set the render template to load the border only if hasBorder is true</t>
         </is>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="13.5">
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>move my view into get_template_part()</t>
+    <row r="146" spans="1:10" ht="13.5">
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>fix table pushing outside the container width</t>
+        </is>
+      </c>
+    </row>
+    <row r="148" spans="1:10" ht="13.5"/>
+    <row r="149" spans="1:10" ht="13.5">
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>fix useEffect infinite loop on couponData</t>
+        </is>
+      </c>
+    </row>
+    <row r="151" spans="1:10" ht="13.5">
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>fix padding excess on bottom button</t>
+        </is>
+      </c>
+    </row>
+    <row r="153" spans="1:10" ht="13.5">
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>add click cursor over trash icon</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
remove margin overWrite on addButton class
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -193,7 +193,7 @@
   <dimension ref="A2:J153"/>
   <sheetViews>
     <sheetView topLeftCell="A135" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C154" sqref="C154"/>
+      <selection activeCell="F152" sqref="F152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -993,6 +993,9 @@
       </c>
     </row>
     <row r="151" spans="1:10" ht="13.5">
+      <c r="A151" t="s">
+        <v>0</v>
+      </c>
       <c r="C151" t="inlineStr">
         <is>
           <t>fix padding excess on bottom button</t>

</xml_diff>

<commit_message>
add coupon route now has cookie/nonce auth
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -190,10 +190,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:J153"/>
+  <dimension ref="A2:J158"/>
   <sheetViews>
     <sheetView topLeftCell="A135" workbookViewId="0" tabSelected="1">
-      <selection activeCell="F152" sqref="F152"/>
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1006,6 +1006,20 @@
       <c r="C153" t="inlineStr">
         <is>
           <t>add click cursor over trash icon</t>
+        </is>
+      </c>
+    </row>
+    <row r="155" spans="1:10" ht="13.5">
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>fix uncheckable checkbox</t>
+        </is>
+      </c>
+    </row>
+    <row r="158" spans="1:10" ht="13.5">
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>add snackbar styling</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix checkbox state switching issue
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -28,12 +28,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>fix uncheckable checkbox</t>
   </si>
   <si>
     <t>admin view</t>
@@ -193,7 +196,7 @@
   <dimension ref="A2:J158"/>
   <sheetViews>
     <sheetView topLeftCell="A135" workbookViewId="0" tabSelected="1">
-      <selection activeCell="I156" sqref="I156"/>
+      <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1016,10 +1019,8 @@
       <c r="A155" t="s">
         <v>1</v>
       </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>fix uncheckable checkbox</t>
-        </is>
+      <c r="C155" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="I155" t="inlineStr">
         <is>
@@ -1151,7 +1152,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -1171,10 +1172,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>2</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1183,7 +1184,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="I20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K20" s="7" t="inlineStr">
         <is>
@@ -1194,10 +1195,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -1232,16 +1233,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" t="s">
         <v>6</v>
       </c>
-      <c r="I26" t="s">
-        <v>5</v>
-      </c>
       <c r="K26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -2169,7 +2170,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -2179,7 +2180,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>

</xml_diff>

<commit_message>
add coupon border radius
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -196,7 +196,7 @@
   <dimension ref="A2:J158"/>
   <sheetViews>
     <sheetView topLeftCell="A135" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C155" sqref="C155"/>
+      <selection activeCell="J150" sqref="J150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -997,6 +997,11 @@
           <t>fix useEffect infinite loop on couponData</t>
         </is>
       </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>I used lodashe's isEqual. It worked perfectly</t>
+        </is>
+      </c>
     </row>
     <row r="151" spans="1:10" ht="13.5">
       <c r="A151" t="s">
@@ -1017,9 +1022,9 @@
     </row>
     <row r="155" spans="1:10" ht="13.5">
       <c r="A155" t="s">
-        <v>1</v>
-      </c>
-      <c r="C155" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C155" t="s">
         <v>2</v>
       </c>
       <c r="I155" t="inlineStr">

</xml_diff>

<commit_message>
fix duplicate record detection
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -28,12 +28,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>2 coupons added to same page</t>
   </si>
   <si>
     <t>fix uncheckable checkbox</t>
@@ -195,8 +198,8 @@
   </sheetPr>
   <dimension ref="A2:J158"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0" tabSelected="1">
-      <selection activeCell="J150" sqref="J150"/>
+    <sheetView topLeftCell="A72" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -657,6 +660,13 @@
         </is>
       </c>
     </row>
+    <row r="79" spans="1:10" ht="13.5">
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>handle blank fields</t>
+        </is>
+      </c>
+    </row>
     <row r="80" spans="1:10" ht="13.5">
       <c r="C80" t="inlineStr">
         <is>
@@ -665,10 +675,11 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="13.5">
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>2 coupons added to same page</t>
-        </is>
+      <c r="A82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
       </c>
       <c r="I82" t="inlineStr">
         <is>
@@ -708,6 +719,9 @@
     </row>
     <row r="89" spans="1:10" ht="13.5"/>
     <row r="90" spans="1:10" ht="13.5">
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
       <c r="B90" t="inlineStr">
         <is>
           <t>add border radius</t>
@@ -1025,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="C155" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I155" t="inlineStr">
         <is>
@@ -1157,7 +1171,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -1177,10 +1191,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1189,7 +1203,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="I20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K20" s="7" t="inlineStr">
         <is>
@@ -1200,10 +1214,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -1238,16 +1252,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
         <v>7</v>
       </c>
-      <c r="I26" t="s">
-        <v>6</v>
-      </c>
       <c r="K26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -2175,7 +2189,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -2185,7 +2199,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>

</xml_diff>

<commit_message>
add enforcement for hits to qualify only after row create date of target
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -33,10 +33,10 @@
     <t>x</t>
   </si>
   <si>
-    <t>/</t>
+    <t>2 coupons added to same page</t>
   </si>
   <si>
-    <t>2 coupons added to same page</t>
+    <t>old visits not counted towards displayThreshold</t>
   </si>
   <si>
     <t>fix uncheckable checkbox</t>
@@ -196,10 +196,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:J160"/>
+  <dimension ref="A2:J163"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0" tabSelected="1">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView topLeftCell="A65" workbookViewId="0" tabSelected="1">
+      <selection activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -480,7 +480,7 @@
     </row>
     <row r="33" spans="1:10" ht="13.5">
       <c r="A33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -620,6 +620,9 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="13.5">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
       <c r="B64" t="inlineStr">
         <is>
           <t>fix the backgrounds only covering text</t>
@@ -662,7 +665,7 @@
     </row>
     <row r="79" spans="1:10" ht="13.5">
       <c r="A79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -671,6 +674,9 @@
       </c>
     </row>
     <row r="80" spans="1:10" ht="13.5">
+      <c r="A80" t="s">
+        <v>0</v>
+      </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>coupon passes view limit</t>
@@ -682,19 +688,17 @@
         <v>0</v>
       </c>
       <c r="C82" t="s">
+        <v>1</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>one should be rejected</t>
+        </is>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="13.5">
+      <c r="C84" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>one should be rejected</t>
-        </is>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="13.5">
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>old visits not counted towards displayThreshold</t>
-        </is>
       </c>
     </row>
     <row r="86" spans="1:10" ht="13.5">
@@ -1031,6 +1035,9 @@
       </c>
     </row>
     <row r="153" spans="1:10" ht="13.5">
+      <c r="A153" t="s">
+        <v>0</v>
+      </c>
       <c r="C153" t="inlineStr">
         <is>
           <t>add click cursor over trash icon</t>
@@ -1061,6 +1068,13 @@
       <c r="C160" t="inlineStr">
         <is>
           <t>fix snackbar jamming without autoClosing</t>
+        </is>
+      </c>
+    </row>
+    <row r="163" spans="1:10" ht="13.5">
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>add forced table column wrapping on a certain pixel width</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
wip adding popover to url field
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -28,18 +28,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>2 coupons added to same page</t>
   </si>
   <si>
     <t>old visits not counted towards displayThreshold</t>
   </si>
   <si>
-    <t>fix uncheckable checkbox</t>
+    <t>fix table pushing outside the container width</t>
   </si>
   <si>
     <t>admin view</t>
@@ -196,10 +193,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:J163"/>
+  <dimension ref="A2:J167"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0" tabSelected="1">
-      <selection activeCell="I87" sqref="I87"/>
+    <sheetView topLeftCell="A149" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -687,18 +684,23 @@
       <c r="A82" t="s">
         <v>0</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2 coupons added to same page</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>one should be rejected</t>
+        </is>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="13.5">
+      <c r="A84" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
         <v>1</v>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>one should be rejected</t>
-        </is>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="13.5">
-      <c r="C84" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="13.5">
@@ -1001,13 +1003,7 @@
         </is>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="13.5">
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>fix table pushing outside the container width</t>
-        </is>
-      </c>
-    </row>
+    <row r="146" spans="1:10" ht="13.5"/>
     <row r="148" spans="1:10" ht="13.5"/>
     <row r="149" spans="1:10" ht="13.5">
       <c r="A149" t="s">
@@ -1048,8 +1044,10 @@
       <c r="A155" t="s">
         <v>0</v>
       </c>
-      <c r="C155" t="s">
-        <v>3</v>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>fix uncheckable checkbox</t>
+        </is>
       </c>
       <c r="I155" t="inlineStr">
         <is>
@@ -1071,10 +1069,29 @@
         </is>
       </c>
     </row>
+    <row r="162" spans="1:10" ht="13.5">
+      <c r="C162" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="163" spans="1:10" ht="13.5">
       <c r="C163" t="inlineStr">
         <is>
-          <t>add forced table column wrapping on a certain pixel width</t>
+          <t>hide too many field chars</t>
+        </is>
+      </c>
+    </row>
+    <row r="164" spans="1:10" ht="13.5">
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>add a popover onHover</t>
+        </is>
+      </c>
+    </row>
+    <row r="167" spans="1:10" ht="13.5">
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>move over to https://www.npmjs.com/package/react-paginate</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1212,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -1215,10 +1232,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1227,7 +1244,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="I20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K20" s="7" t="inlineStr">
         <is>
@@ -1238,10 +1255,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -1276,16 +1293,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
       <c r="I26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" t="s">
         <v>7</v>
-      </c>
-      <c r="K26" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -2213,7 +2230,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -2223,7 +2240,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>

</xml_diff>

<commit_message>
wip new pagination shows but unstyled. refactored out front data filtering
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -28,15 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>old visits not counted towards displayThreshold</t>
-  </si>
-  <si>
-    <t>fix table pushing outside the container width</t>
   </si>
   <si>
     <t>admin view</t>
@@ -193,10 +187,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:J167"/>
+  <dimension ref="A2:J173"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView topLeftCell="A155" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -699,8 +693,10 @@
       <c r="A84" t="s">
         <v>0</v>
       </c>
-      <c r="C84" t="s">
-        <v>1</v>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>old visits not counted towards displayThreshold</t>
+        </is>
       </c>
     </row>
     <row r="86" spans="1:10" ht="13.5">
@@ -1070,11 +1066,16 @@
       </c>
     </row>
     <row r="162" spans="1:10" ht="13.5">
-      <c r="C162" t="s">
-        <v>2</v>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>fix table pushing outside the container width</t>
+        </is>
       </c>
     </row>
     <row r="163" spans="1:10" ht="13.5">
+      <c r="A163" t="s">
+        <v>0</v>
+      </c>
       <c r="C163" t="inlineStr">
         <is>
           <t>hide too many field chars</t>
@@ -1082,16 +1083,81 @@
       </c>
     </row>
     <row r="164" spans="1:10" ht="13.5">
+      <c r="A164" t="s">
+        <v>0</v>
+      </c>
       <c r="C164" t="inlineStr">
         <is>
           <t>add a popover onHover</t>
         </is>
       </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>used tooltips</t>
+        </is>
+      </c>
+    </row>
+    <row r="165" spans="1:10" ht="13.5">
+      <c r="A165" t="s">
+        <v>0</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>configure css to ellipsis the text overflow</t>
+        </is>
+      </c>
+    </row>
+    <row r="166" spans="1:10" ht="13.5">
+      <c r="A166" t="s">
+        <v>0</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>set whitespace to nowrap</t>
+        </is>
+      </c>
     </row>
     <row r="167" spans="1:10" ht="13.5">
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>move over to https://www.npmjs.com/package/react-paginate</t>
+      <c r="A167" t="s">
+        <v>0</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>truncate ending characters</t>
+        </is>
+      </c>
+    </row>
+    <row r="170" spans="1:10" ht="13.5">
+      <c r="A170"/>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>switch to pagination library</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>needs a pagecount and page change</t>
+        </is>
+      </c>
+    </row>
+    <row r="171" spans="1:10" ht="13.5">
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>write front end request, supplying state based offset and 10 limit</t>
+        </is>
+      </c>
+    </row>
+    <row r="172" spans="1:10" ht="13.5">
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>on back end run 2 queries for count, and data</t>
+        </is>
+      </c>
+    </row>
+    <row r="173" spans="1:10" ht="13.5">
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>rewrite the table body render to display the full value of the state variable</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1278,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -1232,10 +1298,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1244,7 +1310,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="I20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K20" s="7" t="inlineStr">
         <is>
@@ -1255,10 +1321,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -1293,16 +1359,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -2230,7 +2296,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -2240,7 +2306,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>

</xml_diff>

<commit_message>
remove axious and outdated ajax function. add Authentication.js
</commit_message>
<xml_diff>
--- a/projectPlansAndNotes.xlsx
+++ b/projectPlansAndNotes.xlsx
@@ -28,9 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
   <si>
     <t>admin view</t>
@@ -187,10 +190,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:J186"/>
+  <dimension ref="A2:J197"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView topLeftCell="A176" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -573,10 +576,8 @@
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
+      <c r="A47" t="s">
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1128,7 +1129,9 @@
       </c>
     </row>
     <row r="170" spans="1:10" ht="13.5">
-      <c r="A170"/>
+      <c r="A170" t="s">
+        <v>1</v>
+      </c>
       <c r="B170" t="inlineStr">
         <is>
           <t>switch to pagination library</t>
@@ -1141,6 +1144,9 @@
       </c>
     </row>
     <row r="171" spans="1:10" ht="13.5">
+      <c r="A171" t="s">
+        <v>1</v>
+      </c>
       <c r="C171" t="inlineStr">
         <is>
           <t>write front end request, supplying state based offset and 10 limit</t>
@@ -1148,6 +1154,9 @@
       </c>
     </row>
     <row r="172" spans="1:10" ht="13.5">
+      <c r="A172" t="s">
+        <v>1</v>
+      </c>
       <c r="C172" t="inlineStr">
         <is>
           <t>on back end run 2 queries for count, and data</t>
@@ -1155,6 +1164,9 @@
       </c>
     </row>
     <row r="173" spans="1:10" ht="13.5">
+      <c r="A173" t="s">
+        <v>1</v>
+      </c>
       <c r="C173" t="inlineStr">
         <is>
           <t>rewrite the table body render to display the full value of the state variable</t>
@@ -1183,6 +1195,9 @@
       </c>
     </row>
     <row r="184" spans="1:10" ht="13.5">
+      <c r="A184" t="s">
+        <v>0</v>
+      </c>
       <c r="B184" t="inlineStr">
         <is>
           <t>create pagination component</t>
@@ -1190,6 +1205,9 @@
       </c>
     </row>
     <row r="185" spans="1:10" ht="13.5">
+      <c r="A185" t="s">
+        <v>0</v>
+      </c>
       <c r="C185" t="inlineStr">
         <is>
           <t>calculate pages needed</t>
@@ -1197,9 +1215,83 @@
       </c>
     </row>
     <row r="186" spans="1:10" ht="13.5">
+      <c r="A186" t="s">
+        <v>0</v>
+      </c>
       <c r="C186" t="inlineStr">
         <is>
           <t>determine currentpage</t>
+        </is>
+      </c>
+    </row>
+    <row r="187" spans="1:10" ht="13.5">
+      <c r="A187" t="s">
+        <v>0</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>set active class</t>
+        </is>
+      </c>
+    </row>
+    <row r="190" spans="1:10" ht="13.5">
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>switch to jwt auth</t>
+        </is>
+      </c>
+    </row>
+    <row r="191" spans="1:10" ht="13.5">
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>download library</t>
+        </is>
+      </c>
+    </row>
+    <row r="192" spans="1:10" ht="13.5">
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>setup .htaccess file</t>
+        </is>
+      </c>
+    </row>
+    <row r="193" spans="1:10" ht="13.5">
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>test requesting a token and logging it</t>
+        </is>
+      </c>
+    </row>
+    <row r="194" spans="1:10" ht="13.5">
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>save the token to a temp cookie</t>
+        </is>
+      </c>
+    </row>
+    <row r="195" spans="1:10" ht="13.5">
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>///</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>test using the token to authorize a load request</t>
+        </is>
+      </c>
+    </row>
+    <row r="196" spans="1:10" ht="13.5">
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>setup token auth on all 3 endpoints</t>
+        </is>
+      </c>
+    </row>
+    <row r="197" spans="1:10" ht="13.5">
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>adjust lifespan of the token</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1412,7 @@
     </row>
     <row r="10" spans="2:11" ht="13.5">
       <c r="J10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="13.5">
@@ -1340,10 +1432,10 @@
     <row r="19" spans="2:11" ht="13.5"/>
     <row r="20" spans="2:11" ht="13.5">
       <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>1</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1352,7 +1444,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="I20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K20" s="7" t="inlineStr">
         <is>
@@ -1363,10 +1455,10 @@
     <row r="21" spans="2:11" ht="13.5"/>
     <row r="22" spans="2:11" ht="13.5">
       <c r="D22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5">
@@ -1401,16 +1493,16 @@
     <row r="25" spans="2:11" ht="13.5"/>
     <row r="26" spans="2:11" ht="13.5">
       <c r="B26" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
         <v>5</v>
       </c>
-      <c r="I26" t="s">
-        <v>4</v>
-      </c>
       <c r="K26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="13.5"/>
@@ -2338,7 +2430,7 @@
         </is>
       </c>
       <c r="F226" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="227" spans="2:11" ht="13.5">
@@ -2348,7 +2440,7 @@
         </is>
       </c>
       <c r="F227" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="228" spans="2:11" ht="13.5"/>

</xml_diff>